<commit_message>
try to fix 2 SBML ODE test cases that aren't validating
</commit_message>
<xml_diff>
--- a/tests/fixtures/verification/cases/semantic/00015/00015-wc_lang.xlsx
+++ b/tests/fixtures/verification/cases/semantic/00015/00015-wc_lang.xlsx
@@ -4737,9 +4737,6 @@
     <t>S2[c]</t>
   </si>
   <si>
-    <t>molar</t>
-  </si>
-  <si>
     <t>reaction_1</t>
   </si>
   <si>
@@ -4894,6 +4891,9 @@
   </si>
   <si>
     <t>k2 * S3[c] * S4[c] * pop_2_conc**2 * vol_c * conv</t>
+  </si>
+  <si>
+    <t>mole / liter</t>
   </si>
 </sst>
 </file>
@@ -5178,12 +5178,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5192,6 +5186,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5787,7 +5787,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B6"/>
+    </sheetView>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -5983,8 +5985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B6"/>
     </sheetView>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="A6" sqref="A6"/>
@@ -6048,16 +6050,16 @@
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>194</v>
-      </c>
       <c r="C3" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -6067,16 +6069,16 @@
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>213</v>
-      </c>
       <c r="D4" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -6162,8 +6164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView showRowColHeaders="0" topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B6"/>
     </sheetView>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="B2" sqref="B2"/>
@@ -6204,13 +6206,13 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="50" t="s">
+      <c r="I2" s="53" t="s">
         <v>86</v>
       </c>
       <c r="J2" s="5"/>
@@ -6265,22 +6267,22 @@
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>169</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>170</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>154</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6293,22 +6295,22 @@
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>184</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>185</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>154</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -6506,14 +6508,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B6"/>
     </sheetView>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="2"/>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="3">
+    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="3">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -6588,19 +6590,19 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -6610,20 +6612,20 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -7508,8 +7510,8 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="2">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="2">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
     <sheetView workbookViewId="3"/>
   </sheetViews>
@@ -7519,7 +7521,7 @@
     <col min="2" max="2" width="28.33203125" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" style="15" customWidth="1"/>
     <col min="6" max="6" width="26.33203125" style="39" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="3" customWidth="1"/>
     <col min="9" max="9" width="2.6640625" customWidth="1"/>
@@ -7580,7 +7582,7 @@
     </row>
     <row r="3" spans="1:11" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B3" s="31"/>
       <c r="C3" s="28"/>
@@ -7591,7 +7593,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -7601,7 +7603,7 @@
     </row>
     <row r="4" spans="1:11" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B4" s="31"/>
       <c r="C4" s="28"/>
@@ -7612,7 +7614,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="44" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K4" s="3"/>
     </row>
@@ -7621,7 +7623,7 @@
         <v>162</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="17">
@@ -7631,7 +7633,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -7641,7 +7643,7 @@
     </row>
     <row r="6" spans="1:11" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
@@ -7649,48 +7651,48 @@
         <v>6.0221408570000002E+23</v>
       </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="51" t="s">
-        <v>198</v>
+      <c r="F6" s="49" t="s">
+        <v>197</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
-      <c r="J6" s="52" t="s">
-        <v>195</v>
+      <c r="J6" s="50" t="s">
+        <v>194</v>
       </c>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>191</v>
-      </c>
       <c r="C7" s="20"/>
-      <c r="D7" s="53">
+      <c r="D7" s="51">
         <v>1</v>
       </c>
       <c r="E7" s="17">
         <v>0</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>218</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="32">
@@ -7700,7 +7702,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -8013,42 +8015,42 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="I2" s="49" t="s">
+      <c r="I2" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="J2" s="50" t="s">
+      <c r="J2" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="K2" s="50" t="s">
+      <c r="K2" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="L2" s="50" t="s">
+      <c r="L2" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="M2" s="50" t="s">
+      <c r="M2" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="N2" s="50" t="s">
+      <c r="N2" s="53" t="s">
         <v>108</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="49" t="s">
+      <c r="Q2" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="R2" s="50" t="s">
+      <c r="R2" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="S2" s="49" t="s">
+      <c r="S2" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="T2" s="50" t="s">
+      <c r="T2" s="53" t="s">
         <v>110</v>
       </c>
       <c r="U2" s="5"/>
@@ -8499,7 +8501,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -8517,7 +8519,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -8928,10 +8930,10 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="53" t="s">
         <v>121</v>
       </c>
       <c r="I2" s="5"/>
@@ -10182,7 +10184,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -10214,7 +10216,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -10246,7 +10248,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -10692,29 +10694,29 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="50" t="s">
+      <c r="I2" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="50" t="s">
+      <c r="J2" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="50" t="s">
+      <c r="K2" s="53" t="s">
         <v>56</v>
       </c>
       <c r="L2" s="5"/>
-      <c r="M2" s="49" t="s">
+      <c r="M2" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="50" t="s">
+      <c r="N2" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="O2" s="50" t="s">
+      <c r="O2" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="P2" s="50" t="s">
+      <c r="P2" s="53" t="s">
         <v>57</v>
       </c>
       <c r="Q2" s="5"/>
@@ -10799,7 +10801,7 @@
         <v>159</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -10816,7 +10818,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L4" s="42" t="s">
         <v>162</v>
@@ -11112,7 +11114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:B6"/>
     </sheetView>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
@@ -11150,22 +11152,22 @@
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="53" t="s">
         <v>69</v>
       </c>
       <c r="I2" s="5"/>
@@ -11243,7 +11245,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="48" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N4" s="3"/>
     </row>
@@ -11271,16 +11273,16 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="48" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -11299,16 +11301,16 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="48" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -11327,7 +11329,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="48" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N7" s="3"/>
     </row>
@@ -11475,8 +11477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A5"/>
+    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B6"/>
     </sheetView>
     <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="C7" sqref="C7"/>
@@ -11548,7 +11550,7 @@
         <v>156</v>
       </c>
       <c r="E3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -11568,7 +11570,7 @@
         <v>156</v>
       </c>
       <c r="E4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -11578,17 +11580,17 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -11598,17 +11600,17 @@
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -11735,8 +11737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="E6" sqref="E6"/>
@@ -11807,7 +11809,7 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="34" t="s">
@@ -11823,7 +11825,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>168</v>
+        <v>220</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -11833,7 +11835,7 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="34" t="s">
@@ -11849,7 +11851,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>168</v>
+        <v>220</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -11859,11 +11861,11 @@
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D5" t="s">
         <v>161</v>
@@ -11875,7 +11877,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>168</v>
+        <v>220</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -11885,11 +11887,11 @@
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D6" t="s">
         <v>161</v>
@@ -11901,7 +11903,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>168</v>
+        <v>220</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>

</xml_diff>

<commit_message>
investigate semantic model 00015-wc_lang.xlsx; add easy-to-read version; test with COPASI, and find that it solves 00015 properly
</commit_message>
<xml_diff>
--- a/tests/fixtures/verification/cases/semantic/00015/00015-wc_lang.xlsx
+++ b/tests/fixtures/verification/cases/semantic/00015/00015-wc_lang.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="340" yWindow="4540" windowWidth="27200" windowHeight="5360" tabRatio="500" firstSheet="4" activeTab="8"/>
-    <workbookView xWindow="480" yWindow="460" windowWidth="34560" windowHeight="4060" tabRatio="500" firstSheet="1" activeTab="5"/>
-    <workbookView xWindow="140" yWindow="15220" windowWidth="30560" windowHeight="6320" tabRatio="500" firstSheet="8" activeTab="16"/>
-    <workbookView xWindow="580" yWindow="9940" windowWidth="30040" windowHeight="5260" tabRatio="500" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="20" yWindow="4560" windowWidth="27200" windowHeight="5360" tabRatio="500" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="25600" windowHeight="4440" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="60" yWindow="14280" windowWidth="30560" windowHeight="6320" tabRatio="500" firstSheet="8" activeTab="12"/>
+    <workbookView xWindow="60" yWindow="9440" windowWidth="30040" windowHeight="5260" tabRatio="500" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -4872,9 +4872,6 @@
     <t>Avogadro * rl_units_conv</t>
   </si>
   <si>
-    <t>k1 * S1[c] * S2[c] * pop_2_conc**2 * vol_c * conv</t>
-  </si>
-  <si>
     <t>Density compt. C</t>
   </si>
   <si>
@@ -4890,10 +4887,13 @@
     <t>1 / molecule</t>
   </si>
   <si>
-    <t>k2 * S3[c] * S4[c] * pop_2_conc**2 * vol_c * conv</t>
-  </si>
-  <si>
     <t>mole / liter</t>
+  </si>
+  <si>
+    <t>k1 * S1[c] * S2[c] * pop_2_conc * pop_2_conc * vol_c * conv</t>
+  </si>
+  <si>
+    <t>k2 * S3[c] * S4[c] * pop_2_conc * pop_2_conc * vol_c * conv</t>
   </si>
 </sst>
 </file>
@@ -6171,7 +6171,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="2"/>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="3"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="3">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6514,9 +6516,11 @@
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="2"/>
-    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="3">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="2">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+    <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="3">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -6599,7 +6603,7 @@
         <v>171</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>179</v>
@@ -6622,7 +6626,7 @@
         <v>171</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>179</v>
@@ -7510,8 +7514,8 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
-    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="2">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="2">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
     <sheetView workbookViewId="3"/>
   </sheetViews>
@@ -7623,7 +7627,7 @@
         <v>162</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="17">
@@ -7683,16 +7687,16 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="22" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>217</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="32">
@@ -7702,7 +7706,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -10647,8 +10651,8 @@
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
-    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
     <sheetView workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
@@ -11825,7 +11829,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -11851,7 +11855,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -11877,7 +11881,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -11903,7 +11907,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>

</xml_diff>

<commit_message>
fix ODE test case wc-lang model 00015
</commit_message>
<xml_diff>
--- a/tests/fixtures/verification/cases/semantic/00015/00015-wc_lang.xlsx
+++ b/tests/fixtures/verification/cases/semantic/00015/00015-wc_lang.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="4560" windowWidth="27200" windowHeight="5360" tabRatio="500" firstSheet="4" activeTab="8"/>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25600" windowHeight="4440" tabRatio="500" firstSheet="1" activeTab="5"/>
-    <workbookView xWindow="60" yWindow="14280" windowWidth="30560" windowHeight="6320" tabRatio="500" firstSheet="8" activeTab="12"/>
-    <workbookView xWindow="60" yWindow="9440" windowWidth="30040" windowHeight="5260" tabRatio="500" firstSheet="9" activeTab="11"/>
+    <workbookView xWindow="340" yWindow="4540" windowWidth="35440" windowHeight="4140" tabRatio="500" firstSheet="4" activeTab="12"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="34560" windowHeight="5020" tabRatio="500" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="460" yWindow="13460" windowWidth="30560" windowHeight="6940" tabRatio="500" firstSheet="8" activeTab="16"/>
+    <workbookView xWindow="420" yWindow="8680" windowWidth="30040" windowHeight="4620" tabRatio="500" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -4737,6 +4737,9 @@
     <t>S2[c]</t>
   </si>
   <si>
+    <t>molar</t>
+  </si>
+  <si>
     <t>reaction_1</t>
   </si>
   <si>
@@ -4836,64 +4839,61 @@
     <t>dist-init-conc-S3[c]</t>
   </si>
   <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S4[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-S4[c]</t>
+  </si>
+  <si>
+    <t>[c]: S3 + S4 ==&gt; S1 + S2</t>
+  </si>
+  <si>
+    <t>litre mole^-1 second^-1</t>
+  </si>
+  <si>
+    <t>abstract_compartment</t>
+  </si>
+  <si>
+    <t>conv</t>
+  </si>
+  <si>
+    <t>Conversion factor for rate laws</t>
+  </si>
+  <si>
+    <t>Avogadro * rl_units_conv</t>
+  </si>
+  <si>
+    <t>k1 * S1[c] * S2[c] * pop_2_conc**2 * vol_c * conv</t>
+  </si>
+  <si>
+    <t>Density compt. C</t>
+  </si>
+  <si>
+    <t>Must equal volume of c in Compartments</t>
+  </si>
+  <si>
+    <t>rl_units_conv</t>
+  </si>
+  <si>
+    <t>Units conversion</t>
+  </si>
+  <si>
+    <t>1 / molecule</t>
+  </si>
+  <si>
+    <t>k2 * S3[c] * S4[c] * pop_2_conc**2 * vol_c * conv</t>
+  </si>
+  <si>
+    <t>test_case_00015_pop_mass_independent</t>
+  </si>
+  <si>
     <t>Basic two reactions with four species in one compartment.</t>
   </si>
   <si>
-    <t>S4</t>
-  </si>
-  <si>
-    <t>S4[c]</t>
-  </si>
-  <si>
-    <t>dist-init-conc-S4[c]</t>
-  </si>
-  <si>
     <t>[c]: S1 + S2 ==&gt; S3 + S4</t>
-  </si>
-  <si>
-    <t>[c]: S3 + S4 ==&gt; S1 + S2</t>
-  </si>
-  <si>
-    <t>litre mole^-1 second^-1</t>
-  </si>
-  <si>
-    <t>test_case_00015_pop_mass_independent</t>
-  </si>
-  <si>
-    <t>abstract_compartment</t>
-  </si>
-  <si>
-    <t>conv</t>
-  </si>
-  <si>
-    <t>Conversion factor for rate laws</t>
-  </si>
-  <si>
-    <t>Avogadro * rl_units_conv</t>
-  </si>
-  <si>
-    <t>Density compt. C</t>
-  </si>
-  <si>
-    <t>Must equal volume of c in Compartments</t>
-  </si>
-  <si>
-    <t>rl_units_conv</t>
-  </si>
-  <si>
-    <t>Units conversion</t>
-  </si>
-  <si>
-    <t>1 / molecule</t>
-  </si>
-  <si>
-    <t>mole / liter</t>
-  </si>
-  <si>
-    <t>k1 * S1[c] * S2[c] * pop_2_conc * pop_2_conc * vol_c * conv</t>
-  </si>
-  <si>
-    <t>k2 * S3[c] * S4[c] * pop_2_conc * pop_2_conc * vol_c * conv</t>
   </si>
 </sst>
 </file>
@@ -5787,9 +5787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B6"/>
-    </sheetView>
+    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -5985,14 +5983,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B6"/>
-    </sheetView>
+    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="2"/>
-    <sheetView workbookViewId="3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6050,16 +6046,16 @@
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>191</v>
-      </c>
       <c r="D3" s="20" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -6069,16 +6065,16 @@
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>212</v>
-      </c>
       <c r="D4" s="20" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -6164,21 +6160,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B6"/>
-    </sheetView>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+    <sheetView showRowColHeaders="0" topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="2"/>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="3">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="14" width="15.6640625" customWidth="1"/>
     <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
   </cols>
@@ -6269,22 +6261,22 @@
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>154</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6297,22 +6289,22 @@
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>154</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -6510,17 +6502,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B6"/>
-    </sheetView>
+    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="2">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="2"/>
     <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="3">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -6594,19 +6582,19 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -6616,20 +6604,20 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -6795,7 +6783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showRowColHeaders="0" workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
@@ -7048,7 +7036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showRowColHeaders="0" workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
@@ -7270,7 +7258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showRowColHeaders="0" workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
@@ -7512,9 +7500,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showRowColHeaders="0" workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
-    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="2">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="2">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
     <sheetView workbookViewId="3"/>
@@ -7525,7 +7513,7 @@
     <col min="2" max="2" width="28.33203125" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="15" customWidth="1"/>
     <col min="6" max="6" width="26.33203125" style="39" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="3" customWidth="1"/>
     <col min="9" max="9" width="2.6640625" customWidth="1"/>
@@ -7586,18 +7574,18 @@
     </row>
     <row r="3" spans="1:11" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B3" s="31"/>
       <c r="C3" s="28"/>
       <c r="D3" s="36">
-        <v>7.5000000000000002E-4</v>
+        <v>750</v>
       </c>
       <c r="E3" s="29">
         <v>0</v>
       </c>
       <c r="F3" s="45" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -7607,18 +7595,18 @@
     </row>
     <row r="4" spans="1:11" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B4" s="31"/>
       <c r="C4" s="28"/>
       <c r="D4" s="36">
-        <v>2.5000000000000001E-4</v>
+        <v>250</v>
       </c>
       <c r="E4" s="29">
         <v>0</v>
       </c>
       <c r="F4" s="44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K4" s="3"/>
     </row>
@@ -7627,7 +7615,7 @@
         <v>162</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="17">
@@ -7637,7 +7625,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -7647,7 +7635,7 @@
     </row>
     <row r="6" spans="1:11" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
@@ -7656,22 +7644,22 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="49" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="50" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="51">
@@ -7681,22 +7669,22 @@
         <v>0</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="32">
@@ -7706,7 +7694,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -8470,8 +8458,8 @@
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
     <sheetView workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
@@ -8479,7 +8467,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="12" width="8.83203125" customWidth="1"/>
     <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
   </cols>
@@ -8505,7 +8493,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -8523,7 +8511,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -10188,7 +10176,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -10220,7 +10208,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -10252,7 +10240,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -10651,7 +10639,7 @@
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
-    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
+    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
     <sheetView workbookViewId="2"/>
@@ -10805,7 +10793,7 @@
         <v>159</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -10822,7 +10810,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="41" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="L4" s="42" t="s">
         <v>162</v>
@@ -11118,9 +11106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B6"/>
-    </sheetView>
+    <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
@@ -11249,7 +11235,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="48" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N4" s="3"/>
     </row>
@@ -11277,16 +11263,16 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="48" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -11305,7 +11291,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="48" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N6" s="3"/>
     </row>
@@ -11333,7 +11319,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="48" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N7" s="3"/>
     </row>
@@ -11481,9 +11467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B6"/>
-    </sheetView>
+    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
     <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
@@ -11554,7 +11538,7 @@
         <v>156</v>
       </c>
       <c r="E3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -11574,7 +11558,7 @@
         <v>156</v>
       </c>
       <c r="E4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -11584,17 +11568,17 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -11614,7 +11598,7 @@
         <v>156</v>
       </c>
       <c r="E6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -11741,10 +11725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+    <sheetView showRowColHeaders="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
     <sheetView workbookViewId="2"/>
@@ -11813,7 +11795,7 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="34" t="s">
@@ -11829,7 +11811,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>218</v>
+        <v>168</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -11839,7 +11821,7 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="34" t="s">
@@ -11855,7 +11837,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>218</v>
+        <v>168</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -11865,11 +11847,11 @@
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="35" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D5" t="s">
         <v>161</v>
@@ -11881,7 +11863,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>218</v>
+        <v>168</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -11907,7 +11889,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>218</v>
+        <v>168</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>

</xml_diff>